<commit_message>
feat(wasm): import sheet view origin for INFO("origin")
</commit_message>
<xml_diff>
--- a/crates/formula-wasm/tests/fixtures/import_styles_cols.xlsx
+++ b/crates/formula-wasm/tests/fixtures/import_styles_cols.xlsx
@@ -44,6 +44,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane topLeftCell="C5"/>
+    </sheetView>
+  </sheetViews>
   <cols>
     <!-- Column B: non-default width + hidden -->
     <col min="2" max="2" width="20" customWidth="1" hidden="1"/>

</xml_diff>

<commit_message>
test(wasm): cover CELL prefix/protect in XLSX import fixture
</commit_message>
<xml_diff>
--- a/crates/formula-wasm/tests/fixtures/import_styles_cols.xlsx
+++ b/crates/formula-wasm/tests/fixtures/import_styles_cols.xlsx
@@ -34,7 +34,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
fix: remove stale pivot cleanup and extend xlsx import CELL coverage
- Drop duplicate pivot pruning block in Engine::delete_sheet that referenced an undefined variable\n  (restores formula-engine compilation).\n- Update wasm xlsx import fixture to use a two-section number format with red parentheses.\n- Assert CELL("color") and CELL("parentheses") are imported correctly.
</commit_message>
<xml_diff>
--- a/crates/formula-wasm/tests/fixtures/import_styles_cols.xlsx
+++ b/crates/formula-wasm/tests/fixtures/import_styles_cols.xlsx
@@ -9,6 +9,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00;[Red](0.00)"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -34,7 +37,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>

</xml_diff>